<commit_message>
fully functional entry deleter and half assed StoreData class
</commit_message>
<xml_diff>
--- a/src/main/resources/demo.xlsx
+++ b/src/main/resources/demo.xlsx
@@ -393,7 +393,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -404,34 +404,12 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rest is working as it should
</commit_message>
<xml_diff>
--- a/src/main/resources/demo.xlsx
+++ b/src/main/resources/demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ilya\Desktop\BookingService\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E54284-F4AF-4CC5-A065-0A68EC2D742C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCF1453-49F9-4C09-A706-1368EBDCC9D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1185" yWindow="0" windowWidth="28500" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -492,7 +492,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C23"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added some code that cleans up first sheet of demo file
</commit_message>
<xml_diff>
--- a/src/main/resources/demo.xlsx
+++ b/src/main/resources/demo.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ilya\Desktop\BookingService\src\main\resources\"/>
     </mc:Choice>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -170,6 +170,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -554,199 +555,188 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
         <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
         <v>18</v>
       </c>
-      <c r="B18" t="s">
-        <v>16</v>
-      </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>23</v>
-      </c>
-      <c r="B23" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" t="s">
         <v>45</v>
       </c>
     </row>
@@ -766,7 +756,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>